<commit_message>
adding gas flow equation. not yet working
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EA6DA4-8F3F-4B54-9C6D-BEABFF55A552}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21801E93-3123-4A36-9784-C1936DEBB8D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10752" yWindow="2772" windowWidth="19704" windowHeight="13380" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="0" yWindow="204" windowWidth="23040" windowHeight="12204" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>id</t>
   </si>
@@ -81,9 +81,6 @@
     <t>distance</t>
   </si>
   <si>
-    <t>flow_k</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -93,18 +90,9 @@
     <t>gas turbine</t>
   </si>
   <si>
-    <t>gas compressor</t>
-  </si>
-  <si>
-    <t>gas processing</t>
-  </si>
-  <si>
     <t>electric load</t>
   </si>
   <si>
-    <t>wind generator</t>
-  </si>
-  <si>
     <t>heat pump</t>
   </si>
   <si>
@@ -144,24 +132,12 @@
     <t>curve_crude</t>
   </si>
   <si>
-    <t>gas export</t>
-  </si>
-  <si>
     <t>co2intensity</t>
   </si>
   <si>
-    <t>el export</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
-    <t>diesel aggregator backup</t>
-  </si>
-  <si>
-    <t>gas compressor (gas)</t>
-  </si>
-  <si>
     <t>coord_z</t>
   </si>
   <si>
@@ -184,6 +160,45 @@
   </si>
   <si>
     <t>export node</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>wind turb</t>
+  </si>
+  <si>
+    <t>diesel backup</t>
+  </si>
+  <si>
+    <t>gas EXPORT</t>
+  </si>
+  <si>
+    <t>el EXPORT</t>
+  </si>
+  <si>
+    <t>compressor1</t>
+  </si>
+  <si>
+    <t>compressor</t>
+  </si>
+  <si>
+    <t>separator</t>
+  </si>
+  <si>
+    <t>nodeFrom</t>
+  </si>
+  <si>
+    <t>nodeTo</t>
+  </si>
+  <si>
+    <t>pressureFrom</t>
+  </si>
+  <si>
+    <t>pressureTo</t>
+  </si>
+  <si>
+    <t>gasflow_k</t>
   </si>
 </sst>
 </file>
@@ -227,10 +242,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,10 +580,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -584,7 +600,7 @@
         <v>0.1</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -631,7 +647,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>-1.2</v>
@@ -643,7 +659,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -654,26 +670,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A70904-C380-433D-9493-9658C938F213}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -691,10 +707,16 @@
         <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -708,7 +730,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="F2">
         <v>1E-3</v>
@@ -720,7 +742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -734,7 +756,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="F3">
         <v>1E-3</v>
@@ -746,7 +768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -760,7 +782,7 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="F4">
         <v>1E-3</v>
@@ -772,38 +794,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -814,16 +830,25 @@
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <v>100</v>
+      </c>
+      <c r="K6">
+        <v>95</v>
+      </c>
+      <c r="L6">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -834,16 +859,25 @@
       <c r="H7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7">
+        <v>400</v>
+      </c>
+      <c r="L7">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
         <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -853,6 +887,44 @@
       </c>
       <c r="H8">
         <v>1</v>
+      </c>
+      <c r="J8">
+        <v>400</v>
+      </c>
+      <c r="K8">
+        <v>395</v>
+      </c>
+      <c r="L8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>200</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>400</v>
+      </c>
+      <c r="K9">
+        <v>395</v>
+      </c>
+      <c r="L9">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>
@@ -865,7 +937,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,46 +953,46 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" t="s">
-        <v>30</v>
-      </c>
       <c r="L1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" t="s">
-        <v>45</v>
-      </c>
       <c r="O1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -928,7 +1000,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -957,19 +1029,22 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="E3" s="2">
-        <v>-0.45</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
         <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0.45</v>
       </c>
       <c r="K3">
         <v>40</v>
@@ -986,7 +1061,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1012,8 +1087,8 @@
       <c r="K4">
         <v>100</v>
       </c>
-      <c r="N4">
-        <v>500</v>
+      <c r="N4" s="3">
+        <v>10000000000</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -1024,13 +1099,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1050,8 +1125,8 @@
       <c r="K5">
         <v>50</v>
       </c>
-      <c r="N5">
-        <v>500</v>
+      <c r="N5" s="3">
+        <v>10000000000</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -1062,7 +1137,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1088,8 +1163,8 @@
       <c r="K6">
         <v>100</v>
       </c>
-      <c r="N6">
-        <v>500</v>
+      <c r="N6" s="3">
+        <v>10000000000</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -1100,7 +1175,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1129,13 +1204,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E8">
         <v>-0.4</v>
@@ -1153,10 +1228,10 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -1164,7 +1239,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1190,7 +1265,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1219,7 +1294,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1245,13 +1320,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1272,15 +1347,15 @@
         <v>300</v>
       </c>
       <c r="O12">
-        <v>200</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1301,7 +1376,7 @@
         <v>0.25</v>
       </c>
       <c r="N13">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="O13">
         <v>10</v>
@@ -1309,10 +1384,10 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1344,7 +1419,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1397,6 +1472,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068757AD89D0841429F5831BBC6267AC1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e521892cf07d8fee7d1fab9fe3aaa83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c" xmlns:ns4="53f6e7f0-9e34-4545-9b50-e54ccadfb78a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ffc55c83d6521c05fad87c69f289641" ns3:_="" ns4:_="">
     <xsd:import namespace="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c"/>
@@ -1605,15 +1689,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1621,6 +1696,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1016DCAE-9D9F-40DE-A38A-1587953D2A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1639,14 +1722,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
in-out change. Working version.
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21801E93-3123-4A36-9784-C1936DEBB8D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26D6D79-5FEE-4A0C-B1AA-0509E308F46E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="204" windowWidth="23040" windowHeight="12204" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="56">
   <si>
     <t>id</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>gasflow_k</t>
+  </si>
+  <si>
+    <t>p_ratio</t>
   </si>
 </sst>
 </file>
@@ -673,7 +676,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,10 +937,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB3A90-DDA6-4778-8302-DAD5F7252115}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,7 +951,7 @@
     <col min="5" max="10" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -994,8 +997,11 @@
       <c r="O1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1024,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1056,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1093,8 +1099,11 @@
       <c r="O4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1131,8 +1140,11 @@
       <c r="O5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1155,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1169,8 +1181,11 @@
       <c r="O6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1193,13 +1208,13 @@
         <v>40</v>
       </c>
       <c r="N7">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="O7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1231,10 +1246,10 @@
         <v>400</v>
       </c>
       <c r="O8">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1260,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1286,10 +1301,10 @@
         <v>10</v>
       </c>
       <c r="O10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1315,7 +1330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1347,10 +1362,10 @@
         <v>300</v>
       </c>
       <c r="O12">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1379,10 +1394,10 @@
         <v>300</v>
       </c>
       <c r="O13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1411,10 +1426,10 @@
         <v>700</v>
       </c>
       <c r="O14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1422,7 +1437,7 @@
         <v>44</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1472,15 +1487,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068757AD89D0841429F5831BBC6267AC1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e521892cf07d8fee7d1fab9fe3aaa83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c" xmlns:ns4="53f6e7f0-9e34-4545-9b50-e54ccadfb78a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ffc55c83d6521c05fad87c69f289641" ns3:_="" ns4:_="">
     <xsd:import namespace="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c"/>
@@ -1689,6 +1695,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1696,14 +1711,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1016DCAE-9D9F-40DE-A38A-1587953D2A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1722,6 +1729,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
preliminary gas flow and pressure constraints.
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26D6D79-5FEE-4A0C-B1AA-0509E308F46E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B7D72B-AFEC-4A6B-81AD-11655A2850F1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>id</t>
   </si>
@@ -192,16 +192,13 @@
     <t>nodeTo</t>
   </si>
   <si>
-    <t>pressureFrom</t>
-  </si>
-  <si>
-    <t>pressureTo</t>
-  </si>
-  <si>
     <t>gasflow_k</t>
   </si>
   <si>
-    <t>p_ratio</t>
+    <t>gaspressure_in</t>
+  </si>
+  <si>
+    <t>gaspressure_out</t>
   </si>
 </sst>
 </file>
@@ -564,15 +561,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052C0DB0-0590-4B7A-AC1E-E28475B8C302}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,8 +585,14 @@
       <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -605,8 +608,14 @@
       <c r="E2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>39</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -619,8 +628,14 @@
       <c r="D3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -633,8 +648,14 @@
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -647,8 +668,14 @@
       <c r="D5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -663,6 +690,12 @@
       </c>
       <c r="E6" t="s">
         <v>41</v>
+      </c>
+      <c r="F6">
+        <v>99</v>
+      </c>
+      <c r="G6">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -673,15 +706,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A70904-C380-433D-9493-9658C938F213}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -712,14 +745,8 @@
       <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -745,7 +772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -771,7 +798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -797,7 +824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -814,7 +841,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -834,16 +861,10 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>100</v>
-      </c>
-      <c r="K6">
-        <v>95</v>
-      </c>
-      <c r="L6">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -863,16 +884,10 @@
         <v>1</v>
       </c>
       <c r="J7">
-        <v>100</v>
-      </c>
-      <c r="K7">
-        <v>400</v>
-      </c>
-      <c r="L7">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -892,16 +907,10 @@
         <v>1</v>
       </c>
       <c r="J8">
-        <v>400</v>
-      </c>
-      <c r="K8">
-        <v>395</v>
-      </c>
-      <c r="L8">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -921,13 +930,7 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>400</v>
-      </c>
-      <c r="K9">
-        <v>395</v>
-      </c>
-      <c r="L9">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -937,10 +940,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB3A90-DDA6-4778-8302-DAD5F7252115}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,7 +954,7 @@
     <col min="5" max="10" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -997,11 +1000,8 @@
       <c r="O1" t="s">
         <v>38</v>
       </c>
-      <c r="P1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1099,11 +1099,8 @@
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1140,11 +1137,8 @@
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1181,11 +1175,8 @@
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1214,7 +1205,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1249,7 +1240,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1275,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1304,7 +1295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1330,7 +1321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1365,7 +1356,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1397,7 +1388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1429,7 +1420,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
added compressor model. seems to work, but energy flow plot not correct
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B7D72B-AFEC-4A6B-81AD-11655A2850F1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A313614D-8B2F-46DD-B3B9-4292262ABC8B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
   <si>
     <t>id</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>gaspressure_out</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>compressor_el</t>
   </si>
 </sst>
 </file>
@@ -708,7 +714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A70904-C380-433D-9493-9658C938F213}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -940,10 +946,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB3A90-DDA6-4778-8302-DAD5F7252115}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:Q1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,7 +960,7 @@
     <col min="5" max="10" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1000,8 +1006,11 @@
       <c r="O1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1030,7 +1039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1062,7 +1071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1099,8 +1108,11 @@
       <c r="O4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1138,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1176,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1205,7 +1217,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1240,7 +1252,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1266,7 +1278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1295,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1321,7 +1333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1356,7 +1368,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1388,7 +1400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1420,7 +1432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
started reformulating -not working yet (vardeviceflow instead of dispatchin/out)
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A313614D-8B2F-46DD-B3B9-4292262ABC8B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3267632A-C392-4850-B42A-303EE0D7CB6C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="node" sheetId="1" r:id="rId1"/>
     <sheet name="edge" sheetId="2" r:id="rId2"/>
     <sheet name="device" sheetId="3" r:id="rId3"/>
-    <sheet name="hub" sheetId="4" r:id="rId4"/>
+    <sheet name="devicemodel" sheetId="5" r:id="rId4"/>
+    <sheet name="hub" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -205,6 +206,27 @@
   </si>
   <si>
     <t>compressor_el</t>
+  </si>
+  <si>
+    <t>source_el</t>
+  </si>
+  <si>
+    <t>sink_el</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>gasturbine</t>
+  </si>
+  <si>
+    <t>el,gas</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
@@ -949,7 +971,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1038,6 +1060,9 @@
       <c r="O2">
         <v>0</v>
       </c>
+      <c r="P2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1070,6 +1095,9 @@
       <c r="O3">
         <v>0</v>
       </c>
+      <c r="P3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1149,6 +1177,9 @@
       <c r="O5">
         <v>0</v>
       </c>
+      <c r="P5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1187,6 +1218,9 @@
       <c r="O6">
         <v>0</v>
       </c>
+      <c r="P6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1216,6 +1250,9 @@
       <c r="O7">
         <v>100</v>
       </c>
+      <c r="P7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1251,6 +1288,9 @@
       <c r="O8">
         <v>200</v>
       </c>
+      <c r="P8" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1277,6 +1317,9 @@
       <c r="O9">
         <v>0</v>
       </c>
+      <c r="P9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1306,6 +1349,9 @@
       <c r="O10">
         <v>0</v>
       </c>
+      <c r="P10" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1332,6 +1378,9 @@
       <c r="O11">
         <v>0</v>
       </c>
+      <c r="P11" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1367,6 +1416,9 @@
       <c r="O12">
         <v>100</v>
       </c>
+      <c r="P12" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1399,6 +1451,9 @@
       <c r="O13">
         <v>0</v>
       </c>
+      <c r="P13" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1431,6 +1486,9 @@
       <c r="O14">
         <v>10</v>
       </c>
+      <c r="P14" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1462,6 +1520,9 @@
       </c>
       <c r="O15">
         <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1470,6 +1531,73 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD106E9-9D7B-4653-84AD-6149C6024DF6}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A00782-5A24-4221-8CB0-9FD918161442}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
reformulated with deviceFlow variables instead of fixed dispatch factors. Diffrent constraints depending on device model. E.g. Compressor electric demand given by pressure difference
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3267632A-C392-4850-B42A-303EE0D7CB6C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09807BC5-C23D-4BA3-9605-94025F4D0528}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="3612" yWindow="3168" windowWidth="23040" windowHeight="12204" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
     <sheet name="edge" sheetId="2" r:id="rId2"/>
     <sheet name="device" sheetId="3" r:id="rId3"/>
-    <sheet name="devicemodel" sheetId="5" r:id="rId4"/>
-    <sheet name="hub" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>id</t>
   </si>
@@ -97,27 +95,6 @@
     <t>heat pump</t>
   </si>
   <si>
-    <t>out_el</t>
-  </si>
-  <si>
-    <t>out_gas</t>
-  </si>
-  <si>
-    <t>out_heat</t>
-  </si>
-  <si>
-    <t>in_el</t>
-  </si>
-  <si>
-    <t>in_gas</t>
-  </si>
-  <si>
-    <t>in_heat</t>
-  </si>
-  <si>
-    <t>nomP</t>
-  </si>
-  <si>
     <t>heat demand</t>
   </si>
   <si>
@@ -133,12 +110,6 @@
     <t>curve_crude</t>
   </si>
   <si>
-    <t>co2intensity</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>coord_z</t>
   </si>
   <si>
@@ -208,25 +179,28 @@
     <t>compressor_el</t>
   </si>
   <si>
-    <t>source_el</t>
-  </si>
-  <si>
     <t>sink_el</t>
   </si>
   <si>
-    <t>in</t>
-  </si>
-  <si>
-    <t>out</t>
-  </si>
-  <si>
     <t>gasturbine</t>
   </si>
   <si>
-    <t>el,gas</t>
-  </si>
-  <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>gen_el</t>
+  </si>
+  <si>
+    <t>compressor_gas</t>
+  </si>
+  <si>
+    <t>sink_gas</t>
+  </si>
+  <si>
+    <t>source_gas</t>
+  </si>
+  <si>
+    <t>eta</t>
   </si>
 </sst>
 </file>
@@ -270,11 +244,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,7 +564,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,16 +580,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -634,13 +606,13 @@
         <v>0.1</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F2">
-        <v>39</v>
+        <v>350</v>
       </c>
       <c r="G2">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -657,10 +629,10 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="G3">
-        <v>40</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -677,10 +649,10 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G4">
-        <v>9</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -697,15 +669,15 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>-1.2</v>
@@ -717,13 +689,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F6">
-        <v>99</v>
+        <v>495</v>
       </c>
       <c r="G6">
-        <v>99</v>
+        <v>495</v>
       </c>
     </row>
   </sheetData>
@@ -737,7 +709,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,13 +719,13 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -771,7 +743,7 @@
         <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -788,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F2">
         <v>1E-3</v>
@@ -814,7 +786,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F3">
         <v>1E-3</v>
@@ -840,7 +812,7 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F4">
         <v>1E-3</v>
@@ -860,13 +832,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>200</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -883,13 +855,13 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -906,13 +878,13 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -929,13 +901,13 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -946,19 +918,19 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -968,10 +940,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB3A90-DDA6-4778-8302-DAD5F7252115}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -979,60 +951,36 @@
     <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="7" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1043,28 +991,16 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>-0.9</v>
-      </c>
-      <c r="K2">
-        <v>5</v>
-      </c>
-      <c r="N2">
-        <v>10</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1074,155 +1010,86 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
-        <v>0</v>
+      <c r="E3">
+        <v>50</v>
       </c>
       <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
       </c>
       <c r="H3">
-        <v>0.45</v>
-      </c>
-      <c r="K3">
-        <v>40</v>
-      </c>
-      <c r="N3">
-        <v>50</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.1</v>
+        <v>1000</v>
       </c>
       <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0.9</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>100</v>
-      </c>
-      <c r="N4" s="3">
-        <v>10000000000</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>52</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0.9</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>50</v>
-      </c>
-      <c r="N5" s="3">
-        <v>10000000000</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0.9</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>100</v>
-      </c>
-      <c r="N6" s="3">
-        <v>10000000000</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1233,66 +1100,39 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>40</v>
-      </c>
-      <c r="N7">
         <v>100</v>
       </c>
-      <c r="O7">
-        <v>100</v>
-      </c>
-      <c r="P7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E8">
-        <v>-0.4</v>
+        <v>400</v>
       </c>
       <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>100</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>400</v>
-      </c>
-      <c r="O8">
         <v>200</v>
       </c>
-      <c r="P8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1303,199 +1143,124 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9">
-        <v>-1</v>
-      </c>
-      <c r="N9">
-        <v>10</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>10</v>
-      </c>
-      <c r="N10">
-        <v>10</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>10</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12">
+        <v>400</v>
+      </c>
+      <c r="F12">
+        <v>220</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>-1</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>200</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="N12">
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13">
         <v>300</v>
       </c>
-      <c r="O12">
-        <v>100</v>
-      </c>
-      <c r="P12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
       <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>200</v>
-      </c>
-      <c r="L13">
-        <v>0.25</v>
-      </c>
-      <c r="N13">
-        <v>300</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>700</v>
       </c>
       <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>100</v>
-      </c>
-      <c r="L14">
-        <v>0.25</v>
-      </c>
-      <c r="N14">
-        <v>700</v>
-      </c>
-      <c r="O14">
         <v>10</v>
       </c>
-      <c r="P14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1504,112 +1269,13 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>20</v>
-      </c>
-      <c r="N15">
-        <v>10</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD106E9-9D7B-4653-84AD-6149C6024DF6}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A00782-5A24-4221-8CB0-9FD918161442}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>12</v>
+      <c r="G15" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated plotting (carriers individually)
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09807BC5-C23D-4BA3-9605-94025F4D0528}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6B5623-35DE-493A-BE86-A7719834C5D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3612" yWindow="3168" windowWidth="23040" windowHeight="12204" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
   <si>
     <t>id</t>
   </si>
@@ -185,9 +185,6 @@
     <t>gasturbine</t>
   </si>
   <si>
-    <t>default</t>
-  </si>
-  <si>
     <t>gen_el</t>
   </si>
   <si>
@@ -201,6 +198,24 @@
   </si>
   <si>
     <t>eta</t>
+  </si>
+  <si>
+    <t>fuelA</t>
+  </si>
+  <si>
+    <t>fuelB</t>
+  </si>
+  <si>
+    <t>sink_heat</t>
+  </si>
+  <si>
+    <t>gasheater</t>
+  </si>
+  <si>
+    <t>heat</t>
+  </si>
+  <si>
+    <t>heatpump</t>
   </si>
 </sst>
 </file>
@@ -564,7 +579,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,10 +955,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB3A90-DDA6-4778-8302-DAD5F7252115}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,7 +969,7 @@
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -977,10 +992,19 @@
         <v>46</v>
       </c>
       <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -997,10 +1021,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1019,11 +1046,17 @@
       <c r="G3" t="s">
         <v>49</v>
       </c>
-      <c r="H3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1046,7 +1079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1063,13 +1096,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H5">
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1089,7 +1122,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1109,7 +1142,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1129,10 +1162,10 @@
         <v>200</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1140,7 +1173,7 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -1149,30 +1182,33 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1189,10 +1225,10 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1212,10 +1248,10 @@
         <v>220</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1232,10 +1268,10 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1255,7 +1291,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1275,7 +1311,27 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1493,18 +1549,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1527,18 +1583,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
tidy up (prior to restructuring)
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6B5623-35DE-493A-BE86-A7719834C5D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C79CDB-D17A-428E-BC59-F0BF8388727D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3612" yWindow="3168" windowWidth="23040" windowHeight="12204" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="9408" yWindow="1236" windowWidth="20040" windowHeight="12408" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -77,9 +77,6 @@
     <t>node4</t>
   </si>
   <si>
-    <t>distance</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -164,9 +161,6 @@
     <t>nodeTo</t>
   </si>
   <si>
-    <t>gasflow_k</t>
-  </si>
-  <si>
     <t>gaspressure_in</t>
   </si>
   <si>
@@ -216,6 +210,21 @@
   </si>
   <si>
     <t>heatpump</t>
+  </si>
+  <si>
+    <t>P=12.71GW for Åsgard</t>
+  </si>
+  <si>
+    <t>length_km</t>
+  </si>
+  <si>
+    <t>diameter_mm</t>
+  </si>
+  <si>
+    <t>temperature_K</t>
+  </si>
+  <si>
+    <t>naturalpressure</t>
   </si>
 </sst>
 </file>
@@ -578,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052C0DB0-0590-4B7A-AC1E-E28475B8C302}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,16 +604,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -621,13 +630,13 @@
         <v>0.1</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2">
-        <v>350</v>
+        <v>2800</v>
       </c>
       <c r="G2">
-        <v>500</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -644,10 +653,10 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>180</v>
+        <v>530</v>
       </c>
       <c r="G3">
-        <v>400</v>
+        <v>2850</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -664,10 +673,10 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>190</v>
+        <v>560</v>
       </c>
       <c r="G4">
-        <v>190</v>
+        <v>560</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -684,15 +693,15 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="G5">
-        <v>200</v>
+        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>-1.2</v>
@@ -701,16 +710,16 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>1.1000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6">
-        <v>495</v>
+        <v>4000</v>
       </c>
       <c r="G6">
-        <v>495</v>
+        <v>4000</v>
       </c>
     </row>
   </sheetData>
@@ -721,26 +730,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A70904-C380-433D-9493-9658C938F213}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -752,16 +761,19 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -787,7 +799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -813,7 +825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -839,7 +851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -847,7 +859,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -856,7 +868,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -875,11 +887,14 @@
       <c r="H6">
         <v>1</v>
       </c>
+      <c r="I6">
+        <v>1000</v>
+      </c>
       <c r="J6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -898,11 +913,14 @@
       <c r="H7">
         <v>1</v>
       </c>
+      <c r="I7">
+        <v>1000</v>
+      </c>
       <c r="J7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -921,11 +939,14 @@
       <c r="H8">
         <v>1</v>
       </c>
+      <c r="I8">
+        <v>1000</v>
+      </c>
       <c r="J8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -933,7 +954,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -944,8 +965,11 @@
       <c r="H9">
         <v>1</v>
       </c>
+      <c r="I9">
+        <v>1000</v>
+      </c>
       <c r="J9">
-        <v>2</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -955,10 +979,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB3A90-DDA6-4778-8302-DAD5F7252115}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -969,70 +993,76 @@
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
         <v>54</v>
       </c>
-      <c r="I1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" t="s">
-        <v>56</v>
-      </c>
       <c r="K1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1044,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -1056,12 +1086,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1073,18 +1103,18 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1096,18 +1126,18 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H5">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1119,15 +1149,15 @@
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1139,38 +1169,38 @@
         <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F8">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1182,18 +1212,18 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1205,15 +1235,15 @@
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1225,58 +1255,64 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>23</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
       <c r="E12">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="F12">
         <v>220</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="L12">
+        <v>600</v>
+      </c>
+      <c r="M12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1288,15 +1324,15 @@
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1311,15 +1347,15 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1331,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1549,18 +1585,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1583,18 +1619,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
starting reformulation with planninghorizon set
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C79CDB-D17A-428E-BC59-F0BF8388727D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AB6270-CCBD-40AE-9AF7-159D6B09F76D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9408" yWindow="1236" windowWidth="20040" windowHeight="12408" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="12336" yWindow="2124" windowWidth="13800" windowHeight="14316" activeTab="3" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
     <sheet name="edge" sheetId="2" r:id="rId2"/>
     <sheet name="device" sheetId="3" r:id="rId3"/>
+    <sheet name="parameters" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
   <si>
     <t>id</t>
   </si>
@@ -225,6 +226,24 @@
   </si>
   <si>
     <t>naturalpressure</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>planning_horizon</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>number of time steps in planning horizon</t>
+  </si>
+  <si>
+    <t>time_delta_minutes</t>
   </si>
 </sst>
 </file>
@@ -587,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052C0DB0-0590-4B7A-AC1E-E28475B8C302}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1368,6 +1387,58 @@
       </c>
       <c r="G16" t="s">
         <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F6EB10-AB47-4D11-878D-7EA50574CBA2}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1585,18 +1656,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1619,18 +1690,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added CO2 minimisation objective, misc improvements
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AB6270-CCBD-40AE-9AF7-159D6B09F76D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0842EB7-101D-4DF4-AFBC-F7F679335784}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12336" yWindow="2124" windowWidth="13800" windowHeight="14316" activeTab="3" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="11520" yWindow="3228" windowWidth="17316" windowHeight="12816" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
     <sheet name="edge" sheetId="2" r:id="rId2"/>
     <sheet name="device" sheetId="3" r:id="rId3"/>
     <sheet name="parameters" sheetId="4" r:id="rId4"/>
+    <sheet name="profiles" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
   <si>
     <t>id</t>
   </si>
@@ -180,15 +181,9 @@
     <t>gasturbine</t>
   </si>
   <si>
-    <t>gen_el</t>
-  </si>
-  <si>
     <t>compressor_gas</t>
   </si>
   <si>
-    <t>sink_gas</t>
-  </si>
-  <si>
     <t>source_gas</t>
   </si>
   <si>
@@ -244,6 +239,27 @@
   </si>
   <si>
     <t>time_delta_minutes</t>
+  </si>
+  <si>
+    <t>timestep</t>
+  </si>
+  <si>
+    <t>curve_const</t>
+  </si>
+  <si>
+    <t>CO2_price</t>
+  </si>
+  <si>
+    <t>export_gas</t>
+  </si>
+  <si>
+    <t>export_el</t>
+  </si>
+  <si>
+    <t>source_el</t>
+  </si>
+  <si>
+    <t>co2em</t>
   </si>
 </sst>
 </file>
@@ -780,13 +796,13 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>14</v>
@@ -998,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB3A90-DDA6-4778-8302-DAD5F7252115}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1012,7 +1028,7 @@
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1035,25 +1051,28 @@
         <v>44</v>
       </c>
       <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
       <c r="L1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="M1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1070,13 +1089,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1095,17 +1114,17 @@
       <c r="G3" t="s">
         <v>47</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1125,10 +1144,10 @@
         <v>45</v>
       </c>
       <c r="H4">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1145,13 +1164,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H5">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1162,16 +1181,16 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F6">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1182,16 +1201,16 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1205,16 +1224,19 @@
         <v>21</v>
       </c>
       <c r="E8">
-        <v>200</v>
+        <v>90</v>
       </c>
       <c r="F8">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1231,13 +1253,13 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1248,16 +1270,16 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1274,10 +1296,10 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1288,25 +1310,25 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="E12">
-        <v>1000</v>
+        <v>220</v>
       </c>
       <c r="F12">
         <v>220</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
-      </c>
-      <c r="L12">
+        <v>49</v>
+      </c>
+      <c r="M12">
         <v>600</v>
       </c>
-      <c r="M12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1320,13 +1342,13 @@
         <v>1000</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1337,16 +1359,16 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="F14">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1356,20 +1378,20 @@
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
       <c r="E15">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1380,13 +1402,36 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F16">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1396,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F6EB10-AB47-4D11-878D-7EA50574CBA2}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1410,10 +1455,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
         <v>14</v>
@@ -1421,24 +1466,397 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>66</v>
-      </c>
-      <c r="B2">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3">
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E6B22F-D4D7-489D-AE2A-F030E504A301}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.76644727800000001</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.77168040699999996</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.95250000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.77691353600000002</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0.92749999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.78214666499999996</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.8869999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.78737979400000002</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0.88300000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.79261292299999997</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.87149999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.797846053</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.82750000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.80806383100000001</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.81828160900000002</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.828499388</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0.83949999999999991</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0.83871716600000001</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0.95250000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.84558434000000005</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0.96500000000000008</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0.85197045199999999</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0.95299999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0.80084982500000002</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0.96050000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0.73382039200000004</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0.99700000000000011</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0.64636604600000003</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1.0525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0.565669058</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>0.47741213300000002</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1.1890000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0.38533609000000002</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1.1519999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>0.41062632700000001</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1.046</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>0.438582729</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0.96899999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>0.46653913200000002</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0.95250000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>0.49449553400000001</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0.52245193700000003</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0.97300000000000009</v>
       </c>
     </row>
   </sheetData>
@@ -1447,6 +1865,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068757AD89D0841429F5831BBC6267AC1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e521892cf07d8fee7d1fab9fe3aaa83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c" xmlns:ns4="53f6e7f0-9e34-4545-9b50-e54ccadfb78a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ffc55c83d6521c05fad87c69f289641" ns3:_="" ns4:_="">
     <xsd:import namespace="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c"/>
@@ -1655,12 +2079,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1671,6 +2089,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1016DCAE-9D9F-40DE-A38A-1587953D2A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1689,15 +2116,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
fixed error in calculation of height factor for gas flow. modified so units for gas flow is MW (energy value) rather than m3/s
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16A0B2F-67BD-4014-A223-010F45F9E9EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A50723E-08F2-4D6F-B06A-6673A36C2230}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6648" yWindow="2796" windowWidth="18888" windowHeight="12204" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="10104" yWindow="3096" windowWidth="18888" windowHeight="12204" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
   <si>
     <t>id</t>
   </si>
@@ -70,15 +70,9 @@
     <t>reactance</t>
   </si>
   <si>
-    <t>node3</t>
-  </si>
-  <si>
     <t>node</t>
   </si>
   <si>
-    <t>node4</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -127,9 +121,6 @@
     <t>include</t>
   </si>
   <si>
-    <t>node1ex</t>
-  </si>
-  <si>
     <t>export node</t>
   </si>
   <si>
@@ -260,6 +251,15 @@
   </si>
   <si>
     <t>co2em</t>
+  </si>
+  <si>
+    <t>export</t>
+  </si>
+  <si>
+    <t>subsea</t>
+  </si>
+  <si>
+    <t>removing makes infeasible - why?</t>
   </si>
 </sst>
 </file>
@@ -623,10 +623,14 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -639,16 +643,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -665,7 +669,7 @@
         <v>0.1</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F2">
         <v>2800</v>
@@ -688,7 +692,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>530</v>
+        <v>580</v>
       </c>
       <c r="G3">
         <v>2850</v>
@@ -696,7 +700,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -708,15 +712,15 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>560</v>
+        <v>590</v>
       </c>
       <c r="G4">
-        <v>560</v>
+        <v>590</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -736,7 +740,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>-1.2</v>
@@ -748,7 +752,7 @@
         <v>0.1</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F6">
         <v>4000</v>
@@ -768,7 +772,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,13 +782,13 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -796,16 +800,16 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -842,7 +846,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -868,7 +872,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -884,6 +888,9 @@
       </c>
       <c r="H4">
         <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -894,7 +901,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -908,16 +915,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -934,7 +941,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -943,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -969,7 +976,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -989,13 +996,13 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1017,7 +1024,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1030,46 +1037,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -1077,19 +1084,19 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H2">
         <v>0.5</v>
@@ -1100,19 +1107,19 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1129,19 +1136,19 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H4">
         <v>1E-3</v>
@@ -1152,19 +1159,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H5">
         <v>4.0000000000000001E-3</v>
@@ -1172,22 +1179,22 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -1195,7 +1202,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1204,10 +1211,10 @@
         <v>50</v>
       </c>
       <c r="F7">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -1215,22 +1222,22 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1241,10 +1248,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -1253,7 +1260,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H9">
         <v>3</v>
@@ -1264,19 +1271,19 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1284,7 +1291,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1296,67 +1303,67 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E12">
-        <v>220</v>
+        <v>5000</v>
       </c>
       <c r="F12">
-        <v>220</v>
+        <v>5000</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M12">
         <v>600</v>
       </c>
       <c r="N12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="F13">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>1000</v>
@@ -1365,7 +1372,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1373,19 +1380,19 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I15">
         <v>30</v>
@@ -1396,7 +1403,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1405,10 +1412,10 @@
         <v>4</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1416,19 +1423,19 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H17">
         <v>3</v>
@@ -1444,7 +1451,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1455,40 +1462,40 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -1511,16 +1518,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added linearised power flow equations for electrical network
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A50723E-08F2-4D6F-B06A-6673A36C2230}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E71088-20E9-4E46-8FE6-38B35C098814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10104" yWindow="3096" windowWidth="18888" windowHeight="12204" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="13668" yWindow="3132" windowWidth="18888" windowHeight="12204" activeTab="1" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="77">
   <si>
     <t>id</t>
   </si>
@@ -260,6 +260,12 @@
   </si>
   <si>
     <t>removing makes infeasible - why?</t>
+  </si>
+  <si>
+    <t>reference_node</t>
+  </si>
+  <si>
+    <t>reference for voltage angles</t>
   </si>
 </sst>
 </file>
@@ -771,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A70904-C380-433D-9493-9658C938F213}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -908,6 +914,12 @@
       </c>
       <c r="E5">
         <v>500</v>
+      </c>
+      <c r="F5">
+        <v>1E-3</v>
+      </c>
+      <c r="G5">
+        <v>0.02</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1023,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB3A90-DDA6-4778-8302-DAD5F7252115}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1448,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F6EB10-AB47-4D11-878D-7EA50574CBA2}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1476,7 +1488,7 @@
         <v>61</v>
       </c>
       <c r="B2">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>63</v>
@@ -1499,6 +1511,17 @@
       </c>
       <c r="B4">
         <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1872,6 +1895,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068757AD89D0841429F5831BBC6267AC1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e521892cf07d8fee7d1fab9fe3aaa83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c" xmlns:ns4="53f6e7f0-9e34-4545-9b50-e54ccadfb78a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ffc55c83d6521c05fad87c69f289641" ns3:_="" ns4:_="">
     <xsd:import namespace="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c"/>
@@ -2080,12 +2109,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2096,6 +2119,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1016DCAE-9D9F-40DE-A38A-1587953D2A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2114,15 +2146,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
added starting/stopping variables (required to include startup costs added ramp rate limit
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6734BE6-B58F-47D8-93B4-A25D133C7558}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838E7C1B-DE4B-42BC-B898-AC65BA0B4E5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13668" yWindow="3132" windowWidth="18888" windowHeight="12204" activeTab="3" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="15804" yWindow="420" windowWidth="18888" windowHeight="16392" activeTab="4" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="82">
   <si>
     <t>id</t>
   </si>
@@ -79,9 +81,6 @@
     <t>gas heater</t>
   </si>
   <si>
-    <t>gas turbine</t>
-  </si>
-  <si>
     <t>electric load</t>
   </si>
   <si>
@@ -266,6 +265,24 @@
   </si>
   <si>
     <t>reference for voltage angles</t>
+  </si>
+  <si>
+    <t>optimisation_timesteps</t>
+  </si>
+  <si>
+    <t>number of timesteps between each optimisation</t>
+  </si>
+  <si>
+    <t>gas turbine2</t>
+  </si>
+  <si>
+    <t>gas turbine1</t>
+  </si>
+  <si>
+    <t>maxRampUp</t>
+  </si>
+  <si>
+    <t>maxRampDown</t>
   </si>
 </sst>
 </file>
@@ -649,16 +666,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -675,7 +692,7 @@
         <v>0.1</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2">
         <v>2800</v>
@@ -706,7 +723,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -726,7 +743,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -746,7 +763,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6">
         <v>-1.2</v>
@@ -758,7 +775,7 @@
         <v>0.1</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6">
         <v>4000</v>
@@ -788,13 +805,13 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -806,13 +823,13 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>12</v>
@@ -852,7 +869,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -878,7 +895,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -896,7 +913,7 @@
         <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -907,7 +924,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -927,10 +944,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -953,7 +970,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1008,7 +1025,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1033,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB3A90-DDA6-4778-8302-DAD5F7252115}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,51 +1064,57 @@
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" t="s">
-        <v>49</v>
-      </c>
       <c r="L1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M1" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="N1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1108,30 +1131,30 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>4.5</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1142,33 +1165,55 @@
       <c r="L3">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="N3">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>4.5</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0.05</v>
+      </c>
+      <c r="M4">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="N4">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>10000</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -1183,251 +1228,254 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>10000</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="E6">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="E7">
         <v>5</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>50</v>
       </c>
       <c r="F7">
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
       <c r="E8">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>5</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="E11">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>10</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13">
         <v>5000</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>5000</v>
       </c>
-      <c r="G12" t="s">
-        <v>46</v>
-      </c>
-      <c r="M12">
+      <c r="G13" t="s">
+        <v>45</v>
+      </c>
+      <c r="O13">
         <v>600</v>
       </c>
-      <c r="N12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="P13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>10000</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>10000</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1000</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>1000</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>20</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>69</v>
+      </c>
+      <c r="I16">
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1438,18 +1486,38 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="E18">
         <v>10</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17">
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18">
         <v>3</v>
       </c>
     </row>
@@ -1460,10 +1528,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F6EB10-AB47-4D11-878D-7EA50574CBA2}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1474,10 +1542,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
         <v>59</v>
-      </c>
-      <c r="B1" t="s">
-        <v>60</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
@@ -1485,29 +1553,29 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2">
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3">
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -1515,13 +1583,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>76</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1533,24 +1612,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E6B22F-D4D7-489D-AE2A-F030E504A301}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>66</v>
-      </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1656,7 +1735,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.56000000000000005</v>
+        <v>0.22</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1670,7 +1749,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.61</v>
+        <v>0.59</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1810,7 +1889,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.38533609000000002</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1824,7 +1903,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.41062632700000001</v>
+        <v>0.06</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1838,7 +1917,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.36</v>
+        <v>0.11</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1852,7 +1931,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.41</v>
+        <v>0.24</v>
       </c>
       <c r="C23">
         <v>1</v>

</xml_diff>

<commit_message>
implemented model update for solveMany (outer loop)
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838E7C1B-DE4B-42BC-B898-AC65BA0B4E5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AA3E4D-8E51-4747-B698-F961BB14607A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15804" yWindow="420" windowWidth="18888" windowHeight="16392" activeTab="4" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="11712" yWindow="612" windowWidth="18888" windowHeight="16392" activeTab="4" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="device" sheetId="3" r:id="rId3"/>
     <sheet name="parameters" sheetId="4" r:id="rId4"/>
     <sheet name="profiles" sheetId="5" r:id="rId5"/>
+    <sheet name="profiles_forecast" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
   <si>
     <t>id</t>
   </si>
@@ -283,6 +284,9 @@
   </si>
   <si>
     <t>maxRampDown</t>
+  </si>
+  <si>
+    <t>curve_wind2</t>
   </si>
 </sst>
 </file>
@@ -1610,15 +1614,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E6B22F-D4D7-489D-AE2A-F030E504A301}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1631,8 +1635,11 @@
       <c r="D1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1645,8 +1652,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>0.58578431366667605</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1659,8 +1669,11 @@
       <c r="D3">
         <v>0.95250000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>0.578431372666666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1673,8 +1686,11 @@
       <c r="D4">
         <v>0.92749999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>0.57107843166666605</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1687,8 +1703,11 @@
       <c r="D5">
         <v>0.8869999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>0.56372549033332398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1701,8 +1720,11 @@
       <c r="D6">
         <v>0.88300000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>0.57598039200006701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1715,8 +1737,11 @@
       <c r="D7">
         <v>0.87149999999999994</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>0.62745098066673299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1729,8 +1754,11 @@
       <c r="D8">
         <v>0.82750000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>0.67892156866666598</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1743,8 +1771,11 @@
       <c r="D9">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>0.73039215666659996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1757,8 +1788,11 @@
       <c r="D10">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>0.75735294099999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1771,8 +1805,11 @@
       <c r="D11">
         <v>0.83949999999999991</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>0.73529411766666597</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1785,8 +1822,11 @@
       <c r="D12">
         <v>0.95250000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>0.71323503563943702</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1799,8 +1839,11 @@
       <c r="D13">
         <v>0.96500000000000008</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>0.69117647066663801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1813,8 +1856,11 @@
       <c r="D14">
         <v>0.95299999999999996</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>0.67401960766665703</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1827,8 +1873,11 @@
       <c r="D15">
         <v>0.96050000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1841,8 +1890,11 @@
       <c r="D16">
         <v>0.99700000000000011</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>0.65931372566667601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1855,8 +1907,11 @@
       <c r="D17">
         <v>1.0525</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>0.65196078466666596</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1869,8 +1924,11 @@
       <c r="D18">
         <v>1.1499999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>0.63235242461224195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1883,8 +1941,11 @@
       <c r="D19">
         <v>1.1890000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>0.58823529366666605</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1897,8 +1958,11 @@
       <c r="D20">
         <v>1.1519999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>0.544117646666609</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1911,8 +1975,11 @@
       <c r="D21">
         <v>1.046</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>0.49999999966666597</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1925,8 +1992,11 @@
       <c r="D22">
         <v>0.96899999999999997</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>0.463235294000028</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1939,8 +2009,11 @@
       <c r="D23">
         <v>0.95250000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>0.44117647066669502</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1953,8 +2026,11 @@
       <c r="D24">
         <v>0.9375</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>0.41911764699999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1966,6 +2042,2897 @@
       </c>
       <c r="D25">
         <v>0.97300000000000009</v>
+      </c>
+      <c r="E25">
+        <v>0.39705908202721202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>0.76644727800000001</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0.37990196066666598</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>0.77168040699999996</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E27">
+        <v>0.37254901966665699</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="E28">
+        <v>0.36519607866666598</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>0.78214666499999996</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0.8869999999999999</v>
+      </c>
+      <c r="E29">
+        <v>0.357843137333342</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="E30">
+        <v>0.345588235000028</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>0.79261292299999997</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0.87149999999999994</v>
+      </c>
+      <c r="E31">
+        <v>0.32352967002724098</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>0.797846053</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0.82750000000000001</v>
+      </c>
+      <c r="E32">
+        <v>0.30147058799999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>0.22</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0.72</v>
+      </c>
+      <c r="E33">
+        <v>0.27941176466666601</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>0.59</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0.72</v>
+      </c>
+      <c r="E34">
+        <v>0.25980392133331398</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>0.79</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0.83949999999999991</v>
+      </c>
+      <c r="E35">
+        <v>0.24509803933333299</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>0.83871716600000001</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E36">
+        <v>0.230392157000019</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0.84558434000000005</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0.96500000000000008</v>
+      </c>
+      <c r="E37">
+        <v>0.215686274333352</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>0.85197045199999999</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="E38">
+        <v>0.20588235299999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>0.80084982500000002</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="E39">
+        <v>0.20588235299999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>0.73382039200000004</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0.99700000000000011</v>
+      </c>
+      <c r="E40">
+        <v>0.20588235299999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>0.64636604600000003</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1.0525</v>
+      </c>
+      <c r="E41">
+        <v>0.20588235299999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>0.565669058</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E42">
+        <v>0.19852941166666599</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>0.41</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1.1890000000000001</v>
+      </c>
+      <c r="E43">
+        <v>0.17647058800002899</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1.1519999999999999</v>
+      </c>
+      <c r="E44">
+        <v>0.15441176466669501</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>0.06</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1.046</v>
+      </c>
+      <c r="E45">
+        <v>0.13235294100002801</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>0.11</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="E46">
+        <v>0.112745098</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>0.24</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E47">
+        <v>9.8039215333314195E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>0.51</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>0.9375</v>
+      </c>
+      <c r="E48">
+        <v>8.3333333333314205E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>0.52245193700000003</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>0.97300000000000009</v>
+      </c>
+      <c r="E49">
+        <v>6.8627278759613206E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>0.76644727800000001</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>5.6372548666666598E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>0.77168040699999996</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E51">
+        <v>4.90196076666762E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="E52">
+        <v>4.1666666666676198E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>0.78214666499999996</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0.8869999999999999</v>
+      </c>
+      <c r="E53">
+        <v>3.43137256666666E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="E54">
+        <v>2.9411764999999899E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>0.79261292299999997</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>0.87149999999999994</v>
+      </c>
+      <c r="E55">
+        <v>2.9411764999999899E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>0.797846053</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0.82750000000000001</v>
+      </c>
+      <c r="E56">
+        <v>2.9411764999999899E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>0.22</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>0.72</v>
+      </c>
+      <c r="E57">
+        <v>2.9411764999999899E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>0.59</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>0.72</v>
+      </c>
+      <c r="E58">
+        <v>3.18627453333237E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>0.79</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>0.83949999999999991</v>
+      </c>
+      <c r="E59">
+        <v>3.9215686333323702E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>0.83871716600000001</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E60">
+        <v>4.65686273333333E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>0.84558434000000005</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>0.96500000000000008</v>
+      </c>
+      <c r="E61">
+        <v>5.3921568333342898E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>0.85197045199999999</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="E62">
+        <v>6.1274423546486503E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>0.80084982500000002</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="E63">
+        <v>6.8627451333342901E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>0.73382039200000004</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>0.99700000000000011</v>
+      </c>
+      <c r="E64">
+        <v>7.5980392333333299E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>0.64636604600000003</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1.0525</v>
+      </c>
+      <c r="E65">
+        <v>8.3333333333323698E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>0.565669058</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E66">
+        <v>8.5784313666666598E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>0.41</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1.1890000000000001</v>
+      </c>
+      <c r="E67">
+        <v>7.8431372666666596E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>1.1519999999999999</v>
+      </c>
+      <c r="E68">
+        <v>7.1078517786844597E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>0.06</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>1.046</v>
+      </c>
+      <c r="E69">
+        <v>6.3725490333323795E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>0.11</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="E70">
+        <v>5.8823528999999999E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>0.24</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E71">
+        <v>5.8823528999999999E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>0.51</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>0.9375</v>
+      </c>
+      <c r="E72">
+        <v>5.8823528999999999E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>0.52245193700000003</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>0.97300000000000009</v>
+      </c>
+      <c r="E73">
+        <v>5.8823528999999999E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>0.76644727800000001</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>5.8823528999999999E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>0.77168040699999996</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E75">
+        <v>5.8823528999999999E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="E76">
+        <v>5.8823528999999999E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>0.78214666499999996</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>0.8869999999999999</v>
+      </c>
+      <c r="E77">
+        <v>5.8823528999999999E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="E78">
+        <v>8.0882352666666504E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>0.79261292299999997</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>0.87149999999999994</v>
+      </c>
+      <c r="E79">
+        <v>0.14705882366657999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>0.797846053</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>0.82750000000000001</v>
+      </c>
+      <c r="E80">
+        <v>0.21323529433333299</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>0.22</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>0.72</v>
+      </c>
+      <c r="E81">
+        <v>0.27941176466666601</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>0.59</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>0.72</v>
+      </c>
+      <c r="E82">
+        <v>0.33823529433333299</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>0.79</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>0.83949999999999991</v>
+      </c>
+      <c r="E83">
+        <v>0.38235294133338998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>0.83871716600000001</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E84">
+        <v>0.42647058833333301</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>0.84558434000000005</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>0.96500000000000008</v>
+      </c>
+      <c r="E85">
+        <v>0.47058823533327598</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>0.85197045199999999</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="E86">
+        <v>0.49264680030614999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>0.80084982500000002</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="E87">
+        <v>0.470588235000028</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>0.73382039200000004</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>0.99700000000000011</v>
+      </c>
+      <c r="E88">
+        <v>0.44852941166666599</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>0.64636604600000003</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>1.0525</v>
+      </c>
+      <c r="E89">
+        <v>0.42647058799999998</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>0.565669058</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E90">
+        <v>0.41176470599999998</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>0.41</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>1.1890000000000001</v>
+      </c>
+      <c r="E91">
+        <v>0.41176470599999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>1.1519999999999999</v>
+      </c>
+      <c r="E92">
+        <v>0.41176470599999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>0.06</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>1.046</v>
+      </c>
+      <c r="E93">
+        <v>0.41176470599999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>0.11</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="E94">
+        <v>0.40441176466669498</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>0.24</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E95">
+        <v>0.382352941</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>0.51</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>0.9375</v>
+      </c>
+      <c r="E96">
+        <v>0.36029411766666603</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>0.52245193700000003</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>0.97300000000000009</v>
+      </c>
+      <c r="E97">
+        <v>0.33823529399997099</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB42B24B-1FF3-4D04-ABC3-37C8B4C6ACE7}">
+  <dimension ref="A1:E97"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.76644727800000001</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0.59769340231754298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.77168040699999996</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.59046130291978205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="E4">
+        <v>0.59813485581324999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.78214666499999996</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.8869999999999999</v>
+      </c>
+      <c r="E5">
+        <v>0.57506542038630204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.56589852559458098</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.79261292299999997</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.87149999999999994</v>
+      </c>
+      <c r="E7">
+        <v>0.63215388971391495</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.797846053</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.82750000000000001</v>
+      </c>
+      <c r="E8">
+        <v>0.65293068330933202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.22</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.72</v>
+      </c>
+      <c r="E9">
+        <v>0.704421761516134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.59</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0.72</v>
+      </c>
+      <c r="E10">
+        <v>0.75814407693264396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.79</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0.83949999999999991</v>
+      </c>
+      <c r="E11">
+        <v>0.74887644594778402</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0.83871716600000001</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E12">
+        <v>0.73160740486585596</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.84558434000000005</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0.96500000000000008</v>
+      </c>
+      <c r="E13">
+        <v>0.68885779365393796</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0.85197045199999999</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="E14">
+        <v>0.67644576094762399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0.80084982500000002</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="E15">
+        <v>0.67611583374164197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0.73382039200000004</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0.99700000000000011</v>
+      </c>
+      <c r="E16">
+        <v>0.66599306136567005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0.64636604600000003</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1.0525</v>
+      </c>
+      <c r="E17">
+        <v>0.66131888718457299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0.565669058</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E18">
+        <v>0.65235631171913999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>0.41</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1.1890000000000001</v>
+      </c>
+      <c r="E19">
+        <v>0.601220644706975</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1.1519999999999999</v>
+      </c>
+      <c r="E20">
+        <v>0.534028917621718</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>0.06</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1.046</v>
+      </c>
+      <c r="E21">
+        <v>0.50956757911247796</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>0.11</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="E22">
+        <v>0.47415122660126902</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>0.24</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E23">
+        <v>0.455974542396479</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>0.51</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0.9375</v>
+      </c>
+      <c r="E24">
+        <v>0.427045275802104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0.52245193700000003</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0.97300000000000009</v>
+      </c>
+      <c r="E25">
+        <v>0.40924897095381402</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>0.76644727800000001</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0.39305910816589501</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>0.77168040699999996</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E27">
+        <v>0.38333713715529499</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="E28">
+        <v>0.37086621732577302</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>0.78214666499999996</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0.8869999999999999</v>
+      </c>
+      <c r="E29">
+        <v>0.37350717950712797</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="E30">
+        <v>0.36130722672349103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>0.79261292299999997</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0.87149999999999994</v>
+      </c>
+      <c r="E31">
+        <v>0.33399145772449701</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>0.797846053</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0.82750000000000001</v>
+      </c>
+      <c r="E32">
+        <v>0.30783347622012402</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>0.22</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0.72</v>
+      </c>
+      <c r="E33">
+        <v>0.28054218343283399</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>0.59</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0.72</v>
+      </c>
+      <c r="E34">
+        <v>0.29630500021846501</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>0.79</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0.83949999999999991</v>
+      </c>
+      <c r="E35">
+        <v>0.27892102176098599</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>0.83871716600000001</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E36">
+        <v>0.25394561185860998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0.84558434000000005</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0.96500000000000008</v>
+      </c>
+      <c r="E37">
+        <v>0.24595995137149701</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>0.85197045199999999</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="E38">
+        <v>0.20541838609917501</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>0.80084982500000002</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="E39">
+        <v>0.20057705816235899</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>0.73382039200000004</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0.99700000000000011</v>
+      </c>
+      <c r="E40">
+        <v>0.202152859632868</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>0.64636604600000003</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1.0525</v>
+      </c>
+      <c r="E41">
+        <v>0.20151845703218099</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>0.565669058</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E42">
+        <v>0.205258501893675</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>0.41</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1.1890000000000001</v>
+      </c>
+      <c r="E43">
+        <v>0.179755845996313</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1.1519999999999999</v>
+      </c>
+      <c r="E44">
+        <v>0.15503588601498899</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>0.06</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1.046</v>
+      </c>
+      <c r="E45">
+        <v>0.132689039007652</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>0.11</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="E46">
+        <v>0.10913959077549</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>0.24</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E47">
+        <v>9.5484050883674607E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>0.51</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>0.9375</v>
+      </c>
+      <c r="E48">
+        <v>8.2550208067668301E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>0.52245193700000003</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>0.97300000000000009</v>
+      </c>
+      <c r="E49">
+        <v>6.8127779299900604E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>0.76644727800000001</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>6.0563196637085301E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>0.77168040699999996</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E51">
+        <v>5.2986512147178297E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="E52">
+        <v>4.4496651640222797E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>0.78214666499999996</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0.8869999999999999</v>
+      </c>
+      <c r="E53">
+        <v>3.6988098472808102E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="E54">
+        <v>2.91923395192153E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>0.79261292299999997</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>0.87149999999999994</v>
+      </c>
+      <c r="E55">
+        <v>2.8697280173846301E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>0.797846053</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0.82750000000000001</v>
+      </c>
+      <c r="E56">
+        <v>2.9218252455743401E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>0.22</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>0.72</v>
+      </c>
+      <c r="E57">
+        <v>2.9357453634942101E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>0.59</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>0.72</v>
+      </c>
+      <c r="E58">
+        <v>3.13152967783909E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>0.79</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>0.83949999999999991</v>
+      </c>
+      <c r="E59">
+        <v>3.8616668512124398E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>0.83871716600000001</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E60">
+        <v>4.6430000188676997E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>0.84558434000000005</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>0.96500000000000008</v>
+      </c>
+      <c r="E61">
+        <v>5.31126783096268E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>0.85197045199999999</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="E62">
+        <v>5.7078217844810299E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>0.80084982500000002</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="E63">
+        <v>6.2963094685152099E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>0.73382039200000004</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>0.99700000000000011</v>
+      </c>
+      <c r="E64">
+        <v>6.92312955732102E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>0.64636604600000003</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1.0525</v>
+      </c>
+      <c r="E65">
+        <v>7.6890690512814899E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>0.565669058</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E66">
+        <v>7.9110035127659906E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>0.41</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1.1890000000000001</v>
+      </c>
+      <c r="E67">
+        <v>7.1915703235945705E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>1.1519999999999999</v>
+      </c>
+      <c r="E68">
+        <v>6.5774681309164307E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>0.06</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>1.046</v>
+      </c>
+      <c r="E69">
+        <v>5.7775439955814301E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>0.11</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="E70">
+        <v>5.9833601450497001E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>0.24</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E71">
+        <v>6.03539128869513E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>0.51</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>0.9375</v>
+      </c>
+      <c r="E72">
+        <v>6.0463136572759799E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>0.52245193700000003</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>0.97300000000000009</v>
+      </c>
+      <c r="E73">
+        <v>6.1322688891674103E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>0.76644727800000001</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>5.9736130819320797E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>0.77168040699999996</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E75">
+        <v>6.0140275239088999E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="E76">
+        <v>5.96531677065925E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>0.78214666499999996</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>0.8869999999999999</v>
+      </c>
+      <c r="E77">
+        <v>5.84714145774759E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="E78">
+        <v>7.8789564915307406E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>0.79261292299999997</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>0.87149999999999994</v>
+      </c>
+      <c r="E79">
+        <v>0.14707776690524499</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>0.797846053</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>0.82750000000000001</v>
+      </c>
+      <c r="E80">
+        <v>0.20729352833268999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>0.22</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>0.72</v>
+      </c>
+      <c r="E81">
+        <v>0.27034418799264398</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>0.59</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>0.72</v>
+      </c>
+      <c r="E82">
+        <v>0.313393018340896</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>0.79</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>0.83949999999999991</v>
+      </c>
+      <c r="E83">
+        <v>0.35574786049351098</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>0.83871716600000001</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E84">
+        <v>0.396922973396374</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>0.84558434000000005</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>0.96500000000000008</v>
+      </c>
+      <c r="E85">
+        <v>0.43854342077059499</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>0.85197045199999999</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="E86">
+        <v>0.47934780589218001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>0.80084982500000002</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="E87">
+        <v>0.46939401898864602</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>0.73382039200000004</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>0.99700000000000011</v>
+      </c>
+      <c r="E88">
+        <v>0.439552109858589</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>0.64636604600000003</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>1.0525</v>
+      </c>
+      <c r="E89">
+        <v>0.417960446402596</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>0.565669058</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E90">
+        <v>0.39828282080507699</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>0.41</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>1.1890000000000001</v>
+      </c>
+      <c r="E91">
+        <v>0.40225898846856201</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>1.1519999999999999</v>
+      </c>
+      <c r="E92">
+        <v>0.40410332094809498</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>0.06</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>1.046</v>
+      </c>
+      <c r="E93">
+        <v>0.41102614392046299</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>0.11</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="E94">
+        <v>0.38888859041332202</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>0.24</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="E95">
+        <v>0.36672851103095599</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>0.51</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>0.9375</v>
+      </c>
+      <c r="E96">
+        <v>0.349249430756434</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>0.52245193700000003</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>0.97300000000000009</v>
+      </c>
+      <c r="E97">
+        <v>0.33338357391509399</v>
       </c>
     </row>
   </sheetData>
@@ -1974,12 +4941,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068757AD89D0841429F5831BBC6267AC1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e521892cf07d8fee7d1fab9fe3aaa83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c" xmlns:ns4="53f6e7f0-9e34-4545-9b50-e54ccadfb78a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ffc55c83d6521c05fad87c69f289641" ns3:_="" ns4:_="">
     <xsd:import namespace="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c"/>
@@ -2188,6 +5149,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2198,15 +5165,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1016DCAE-9D9F-40DE-A38A-1587953D2A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2225,6 +5183,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
continued outer loop added (memory) storage ov simulation results added plots
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AA3E4D-8E51-4747-B698-F961BB14607A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57EF0D9-7A10-4C15-AA96-8396EB40C7CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11712" yWindow="612" windowWidth="18888" windowHeight="16392" activeTab="4" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="11712" yWindow="612" windowWidth="18888" windowHeight="16392" activeTab="5" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
   <si>
     <t>id</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>curve_wind2</t>
+  </si>
+  <si>
+    <t>wind3</t>
   </si>
 </sst>
 </file>
@@ -1616,7 +1619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E6B22F-D4D7-489D-AE2A-F030E504A301}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -3278,15 +3281,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB42B24B-1FF3-4D04-ABC3-37C8B4C6ACE7}">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3302,13 +3303,16 @@
       <c r="E1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.76644727800000001</v>
+        <v>0.91973673359999997</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3319,13 +3323,17 @@
       <c r="E2">
         <v>0.59769340231754298</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <f>MIN(1,MAX(0,B2*(1+0.2*COS(A2*PI()/9))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.77168040699999996</v>
+        <v>0.91670888381259319</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3336,13 +3344,17 @@
       <c r="E3">
         <v>0.59046130291978205</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <f t="shared" ref="F3:G66" si="0">MIN(1,MAX(0,B3*(1+0.2*COS(A3*PI()/9))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.76200000000000001</v>
+        <v>0.87874517313133227</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3353,13 +3365,17 @@
       <c r="E4">
         <v>0.59813485581324999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.78214666499999996</v>
+        <v>0.86036133150000005</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3370,13 +3386,17 @@
       <c r="E5">
         <v>0.57506542038630204</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.94639746465000008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.81100000000000005</v>
+        <v>0.83916573441757625</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3387,13 +3407,17 @@
       <c r="E6">
         <v>0.56589852559458098</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.86830965452600495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.79261292299999997</v>
+        <v>0.76508576506515824</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3404,13 +3428,17 @@
       <c r="E7">
         <v>0.63215388971391495</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.73851461529266349</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.797846053</v>
+        <v>0.71806144770000002</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3421,13 +3449,17 @@
       <c r="E8">
         <v>0.65293068330933202</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.64625530293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.22</v>
+        <v>0.18629404450276499</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3438,13 +3470,17 @@
       <c r="E9">
         <v>0.704421761516134</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.15775214098726445</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.59</v>
+        <v>0.47911627074726276</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -3455,13 +3491,17 @@
       <c r="E10">
         <v>0.75814407693264396</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.38907186592332949</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.79</v>
+        <v>0.63200000000000012</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -3472,13 +3512,17 @@
       <c r="E11">
         <v>0.74887644594778402</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.50560000000000016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.83871716600000001</v>
+        <v>0.681089899636666</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3489,13 +3533,17 @@
       <c r="E12">
         <v>0.73160740486585596</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.55308686908058802</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.84558434000000005</v>
+        <v>0.71603330303091428</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -3506,13 +3554,17 @@
       <c r="E13">
         <v>0.68885779365393796</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.60633063645592244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.85197045199999999</v>
+        <v>0.76677340679999995</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -3523,13 +3575,17 @@
       <c r="E14">
         <v>0.67644576094762399</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.69009606611999985</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.80084982500000002</v>
+        <v>0.77303660246077399</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3540,13 +3596,17 @@
       <c r="E15">
         <v>0.67611583374164197</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.74618932300334428</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.73382039200000004</v>
+        <v>0.75930570676112641</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -3557,13 +3617,17 @@
       <c r="E16">
         <v>0.66599306136567005</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.78567611721536035</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.64636604600000003</v>
+        <v>0.7110026505999999</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -3574,13 +3638,17 @@
       <c r="E17">
         <v>0.66131888718457299</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0.78210291565999979</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.565669058</v>
+        <v>0.65233458570504943</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -3591,13 +3659,17 @@
       <c r="E18">
         <v>0.65235631171913999</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0.75227804259178421</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.41</v>
+        <v>0.48705479490444442</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -3608,13 +3680,17 @@
       <c r="E19">
         <v>0.601220644706975</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0.57859115424246443</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.28000000000000003</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -3625,13 +3701,17 @@
       <c r="E20">
         <v>0.534028917621718</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0.4032</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.06</v>
+        <v>7.1276311449430904E-2</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -3642,13 +3722,17 @@
       <c r="E21">
         <v>0.50956757911247796</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>8.4671876230604584E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.11</v>
+        <v>0.12685297774861753</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3659,13 +3743,17 @@
       <c r="E22">
         <v>0.47415122660126902</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0.14628798148810232</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.24</v>
+        <v>0.26399999999999996</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -3676,13 +3764,17 @@
       <c r="E23">
         <v>0.455974542396479</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0.29039999999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.51</v>
+        <v>0.52771211412202701</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3693,13 +3785,17 @@
       <c r="E24">
         <v>0.427045275802104</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0.54603936351203786</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.52245193700000003</v>
+        <v>0.50430737164427852</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3710,13 +3806,17 @@
       <c r="E25">
         <v>0.40924897095381402</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0.48679296043027293</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.76644727800000001</v>
+        <v>0.68980255020000014</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3727,13 +3827,17 @@
       <c r="E26">
         <v>0.39305910816589501</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0.62082229518000021</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.77168040699999996</v>
+        <v>0.6534521094707717</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3744,13 +3848,17 @@
       <c r="E27">
         <v>0.38333713715529499</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>0.55333743800987989</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.76200000000000001</v>
+        <v>0.61879084459222755</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3761,13 +3869,17 @@
       <c r="E28">
         <v>0.37086621732577302</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0.5024962064975883</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.78214666499999996</v>
+        <v>0.62571733200000001</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -3778,13 +3890,17 @@
       <c r="E29">
         <v>0.37350717950712797</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0.50057386560000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.81100000000000005</v>
+        <v>0.65858185690852566</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -3795,13 +3911,17 @@
       <c r="E30">
         <v>0.36130722672349103</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0.53480895468444112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.79261292299999997</v>
+        <v>0.6711775779583119</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -3812,13 +3932,17 @@
       <c r="E31">
         <v>0.33399145772449701</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>0.568347207170108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.797846053</v>
+        <v>0.7180614476999998</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3829,13 +3953,17 @@
       <c r="E32">
         <v>0.30783347622012402</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>0.64625530292999955</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.22</v>
+        <v>0.21235948018265505</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3846,13 +3974,17 @@
       <c r="E33">
         <v>0.28054218343283399</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0.2049843128338521</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.59</v>
+        <v>0.61049048496469771</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3863,13 +3995,17 @@
       <c r="E34">
         <v>0.29630500021846501</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>0.63169259700412173</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.79</v>
+        <v>0.86900000000000011</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -3880,13 +4016,17 @@
       <c r="E35">
         <v>0.27892102176098599</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>0.95590000000000019</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.83871716600000001</v>
+        <v>0.96721609087255955</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -3897,13 +4037,17 @@
       <c r="E36">
         <v>0.25394561185860998</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.84558434000000005</v>
+        <v>1</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -3914,13 +4058,17 @@
       <c r="E37">
         <v>0.24595995137149701</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.85197045199999999</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -3931,13 +4079,17 @@
       <c r="E38">
         <v>0.20541838609917501</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.80084982500000002</v>
+        <v>0.95136035918203732</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -3948,13 +4100,17 @@
       <c r="E39">
         <v>0.20057705816235899</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.73382039200000004</v>
+        <v>0.8462481987077981</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -3965,13 +4121,17 @@
       <c r="E40">
         <v>0.202152859632868</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>0.97590094473170885</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.64636604600000003</v>
+        <v>0.71100265060000023</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -3982,13 +4142,17 @@
       <c r="E41">
         <v>0.20151845703218099</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>0.78210291566000045</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.565669058</v>
+        <v>0.58531453821685386</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -3999,13 +4163,17 @@
       <c r="E42">
         <v>0.205258501893675</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>0.60564229880151743</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.41</v>
+        <v>0.3957608494313119</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -4016,13 +4184,17 @@
       <c r="E43">
         <v>0.179755845996313</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>0.38201621937217933</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0.28000000000000003</v>
+        <v>0.252</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -4033,13 +4205,17 @@
       <c r="E44">
         <v>0.15503588601498899</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>0.22679999999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.06</v>
+        <v>5.0807466682572272E-2</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -4050,13 +4226,17 @@
       <c r="E45">
         <v>0.132689039007652</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>4.3023311178344861E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0.11</v>
+        <v>8.9326762342710031E-2</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -4067,13 +4247,17 @@
       <c r="E46">
         <v>0.10913959077549</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>7.2538822460281802E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.24</v>
+        <v>0.192</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -4084,13 +4268,17 @@
       <c r="E47">
         <v>9.5484050883674607E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>0.15360000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0.51</v>
+        <v>0.41415135267983727</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -4101,13 +4289,17 @@
       <c r="E48">
         <v>8.2550208067668301E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>0.33631635867948817</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0.52245193700000003</v>
+        <v>0.44240765637288088</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -4118,13 +4310,17 @@
       <c r="E49">
         <v>6.8127779299900604E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>0.37462687102133385</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0.76644727800000001</v>
+        <v>0.68980255019999981</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -4135,13 +4331,17 @@
       <c r="E50">
         <v>6.0563196637085301E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>0.62082229517999965</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.77168040699999996</v>
+        <v>0.74488022771663465</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -4152,13 +4352,17 @@
       <c r="E51">
         <v>5.2986512147178297E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>0.71901080889200997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0.76200000000000001</v>
+        <v>0.78846398227644021</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -4169,13 +4373,17 @@
       <c r="E52">
         <v>4.4496651640222797E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>0.81584704901210325</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.78214666499999996</v>
+        <v>0.86036133150000005</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -4186,13 +4394,17 @@
       <c r="E53">
         <v>3.6988098472808102E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>0.94639746465000008</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.81100000000000005</v>
+        <v>0.93525240867389836</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -4203,13 +4415,17 @@
       <c r="E54">
         <v>2.91923395192153E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0.79261292299999997</v>
+        <v>0.94157542597652977</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -4220,13 +4436,17 @@
       <c r="E55">
         <v>2.8697280173846301E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56">
-        <v>0.797846053</v>
+        <v>0.95741526359999995</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -4237,13 +4457,17 @@
       <c r="E56">
         <v>2.9218252455743401E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0.22</v>
+        <v>0.26134647531458</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -4254,13 +4478,17 @@
       <c r="E57">
         <v>2.9357453634942101E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>0.3104635461788835</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0.59</v>
+        <v>0.68039324428803949</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -4271,13 +4499,17 @@
       <c r="E58">
         <v>3.13152967783909E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>0.78463553707254885</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0.79</v>
+        <v>0.86900000000000033</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -4288,13 +4520,17 @@
       <c r="E59">
         <v>3.8616668512124398E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>0.95590000000000064</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0.83871716600000001</v>
+        <v>0.86784550749077438</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -4305,13 +4541,17 @@
       <c r="E60">
         <v>4.6430000188676997E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>0.89798546566521531</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0.84558434000000005</v>
+        <v>0.81621750405906168</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -4322,13 +4562,17 @@
       <c r="E61">
         <v>5.31126783096268E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>0.78787056762712093</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.85197045199999999</v>
+        <v>0.7667734068000005</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -4339,13 +4583,17 @@
       <c r="E62">
         <v>5.7078217844810299E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>0.69009606612000085</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0.80084982500000002</v>
+        <v>0.67815251335718874</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -4356,13 +4604,17 @@
       <c r="E63">
         <v>6.2963094685152099E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>0.57425352046830014</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0.73382039200000004</v>
+        <v>0.59590727053107562</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -4373,13 +4625,17 @@
       <c r="E64">
         <v>6.92312955732102E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>0.48391333757293092</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0.64636604600000003</v>
+        <v>0.51709283680000007</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -4390,13 +4646,17 @@
       <c r="E65">
         <v>7.6890690512814899E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>0.41367426944000008</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0.565669058</v>
+        <v>0.45935805007809671</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -4407,13 +4667,17 @@
       <c r="E66">
         <v>7.9110035127659906E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>0.37302697608669838</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0.41</v>
+        <v>0.34718435566424366</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -4424,13 +4688,17 @@
       <c r="E67">
         <v>7.1915703235945705E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F67">
+        <f t="shared" ref="F67:G97" si="1">MIN(1,MAX(0,B67*(1+0.2*COS(A67*PI()/9))))</f>
+        <v>0.29399262638535623</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0.28000000000000003</v>
+        <v>0.25200000000000011</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -4441,13 +4709,17 @@
       <c r="E68">
         <v>6.5774681309164307E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>0.22680000000000017</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0.06</v>
+        <v>5.7916221867996803E-2</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -4458,13 +4730,17 @@
       <c r="E69">
         <v>5.7775439955814301E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>5.5904812591050519E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.11</v>
+        <v>0.11382025990867248</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -4475,13 +4751,17 @@
       <c r="E70">
         <v>5.9833601450497001E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>0.11777319605161596</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0.24</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -4492,13 +4772,17 @@
       <c r="E71">
         <v>6.03539128869513E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>0.29040000000000005</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0.51</v>
+        <v>0.58813653319813575</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -4509,13 +4793,17 @@
       <c r="E72">
         <v>6.0463136572759799E-2</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>0.67824427780847418</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.52245193700000003</v>
+        <v>0.62064078298284087</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -4526,13 +4814,17 @@
       <c r="E73">
         <v>6.1322688891674103E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>0.73728309576839357</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0.76644727800000001</v>
+        <v>0.91973673359999997</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -4543,13 +4835,17 @@
       <c r="E74">
         <v>5.9736130819320797E-2</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0.77168040699999996</v>
+        <v>0.9167088838125933</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -4560,13 +4856,17 @@
       <c r="E75">
         <v>6.0140275239088999E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0.76200000000000001</v>
+        <v>0.87874517313133249</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -4577,13 +4877,17 @@
       <c r="E76">
         <v>5.96531677065925E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0.78214666499999996</v>
+        <v>0.86036133150000016</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -4594,13 +4898,17 @@
       <c r="E77">
         <v>5.84714145774759E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>0.94639746465000041</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0.81100000000000005</v>
+        <v>0.83916573441757658</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -4611,13 +4919,17 @@
       <c r="E78">
         <v>7.8789564915307406E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>0.86830965452600573</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0.79261292299999997</v>
+        <v>0.76508576506515813</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -4628,13 +4940,17 @@
       <c r="E79">
         <v>0.14707776690524499</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>0.73851461529266327</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0.797846053</v>
+        <v>0.71806144770000047</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -4645,13 +4961,17 @@
       <c r="E80">
         <v>0.20729352833268999</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F80">
+        <f t="shared" si="1"/>
+        <v>0.64625530293000089</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
       <c r="B81">
-        <v>0.22</v>
+        <v>0.18629404450276499</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -4662,13 +4982,17 @@
       <c r="E81">
         <v>0.27034418799264398</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F81">
+        <f t="shared" si="1"/>
+        <v>0.15775214098726445</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
       <c r="B82">
-        <v>0.59</v>
+        <v>0.47911627074726282</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -4679,13 +5003,17 @@
       <c r="E82">
         <v>0.313393018340896</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F82">
+        <f t="shared" si="1"/>
+        <v>0.3890718659233296</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
       <c r="B83">
-        <v>0.79</v>
+        <v>0.63200000000000012</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -4696,13 +5024,17 @@
       <c r="E83">
         <v>0.35574786049351098</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F83">
+        <f t="shared" si="1"/>
+        <v>0.50560000000000016</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
       <c r="B84">
-        <v>0.83871716600000001</v>
+        <v>0.68108989963666577</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -4713,13 +5045,17 @@
       <c r="E84">
         <v>0.396922973396374</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F84">
+        <f t="shared" si="1"/>
+        <v>0.55308686908058757</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
       <c r="B85">
-        <v>0.84558434000000005</v>
+        <v>0.7160333030309145</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -4730,13 +5066,17 @@
       <c r="E85">
         <v>0.43854342077059499</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F85">
+        <f t="shared" si="1"/>
+        <v>0.60633063645592278</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
       <c r="B86">
-        <v>0.85197045199999999</v>
+        <v>0.76677340680000017</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -4747,13 +5087,17 @@
       <c r="E86">
         <v>0.47934780589218001</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F86">
+        <f t="shared" si="1"/>
+        <v>0.6900960661200003</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0.80084982500000002</v>
+        <v>0.7730366024607741</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -4764,13 +5108,17 @@
       <c r="E87">
         <v>0.46939401898864602</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F87">
+        <f t="shared" si="1"/>
+        <v>0.74618932300334451</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
       <c r="B88">
-        <v>0.73382039200000004</v>
+        <v>0.75930570676112608</v>
       </c>
       <c r="C88">
         <v>1</v>
@@ -4781,13 +5129,17 @@
       <c r="E88">
         <v>0.439552109858589</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F88">
+        <f t="shared" si="1"/>
+        <v>0.78567611721535968</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
       <c r="B89">
-        <v>0.64636604600000003</v>
+        <v>0.71100265059999967</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -4798,13 +5150,17 @@
       <c r="E89">
         <v>0.417960446402596</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F89">
+        <f t="shared" si="1"/>
+        <v>0.78210291565999923</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
       <c r="B90">
-        <v>0.565669058</v>
+        <v>0.65233458570504921</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -4815,13 +5171,17 @@
       <c r="E90">
         <v>0.39828282080507699</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F90">
+        <f t="shared" si="1"/>
+        <v>0.75227804259178366</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0.41</v>
+        <v>0.48705479490444442</v>
       </c>
       <c r="C91">
         <v>1</v>
@@ -4832,13 +5192,17 @@
       <c r="E91">
         <v>0.40225898846856201</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F91">
+        <f t="shared" si="1"/>
+        <v>0.57859115424246443</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
       <c r="B92">
-        <v>0.28000000000000003</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -4849,13 +5213,17 @@
       <c r="E92">
         <v>0.40410332094809498</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F92">
+        <f t="shared" si="1"/>
+        <v>0.4032</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0.06</v>
+        <v>7.1276311449430904E-2</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -4866,13 +5234,17 @@
       <c r="E93">
         <v>0.41102614392046299</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F93">
+        <f t="shared" si="1"/>
+        <v>8.4671876230604584E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0.11</v>
+        <v>0.12685297774861756</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -4883,13 +5255,17 @@
       <c r="E94">
         <v>0.38888859041332202</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F94">
+        <f t="shared" si="1"/>
+        <v>0.14628798148810238</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0.24</v>
+        <v>0.26400000000000012</v>
       </c>
       <c r="C95">
         <v>1</v>
@@ -4900,13 +5276,17 @@
       <c r="E95">
         <v>0.36672851103095599</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F95">
+        <f t="shared" si="1"/>
+        <v>0.29040000000000027</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0.51</v>
+        <v>0.52771211412202645</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -4917,13 +5297,17 @@
       <c r="E96">
         <v>0.349249430756434</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F96">
+        <f t="shared" si="1"/>
+        <v>0.54603936351203664</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0.52245193700000003</v>
+        <v>0.50430737164427875</v>
       </c>
       <c r="C97">
         <v>1</v>
@@ -4933,6 +5317,10 @@
       </c>
       <c r="E97">
         <v>0.33338357391509399</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="1"/>
+        <v>0.48679296043027337</v>
       </c>
     </row>
   </sheetData>
@@ -4941,6 +5329,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068757AD89D0841429F5831BBC6267AC1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e521892cf07d8fee7d1fab9fe3aaa83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c" xmlns:ns4="53f6e7f0-9e34-4545-9b50-e54ccadfb78a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ffc55c83d6521c05fad87c69f289641" ns3:_="" ns4:_="">
     <xsd:import namespace="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c"/>
@@ -5149,12 +5543,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5165,6 +5553,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1016DCAE-9D9F-40DE-A38A-1587953D2A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5183,15 +5580,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
addes electric storage (need to improve usage strategy)
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57EF0D9-7A10-4C15-AA96-8396EB40C7CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327E909B-DD31-40F5-B2B7-84DB7DF41425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11712" yWindow="612" windowWidth="18888" windowHeight="16392" activeTab="5" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="9252" yWindow="252" windowWidth="18888" windowHeight="16392" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="87">
   <si>
     <t>id</t>
   </si>
@@ -290,6 +290,15 @@
   </si>
   <si>
     <t>wind3</t>
+  </si>
+  <si>
+    <t>battery</t>
+  </si>
+  <si>
+    <t>storage_el</t>
+  </si>
+  <si>
+    <t>Emax</t>
   </si>
 </sst>
 </file>
@@ -1057,9 +1066,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB3A90-DDA6-4778-8302-DAD5F7252115}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -1071,7 +1080,7 @@
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1118,10 +1127,13 @@
         <v>57</v>
       </c>
       <c r="P1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1144,7 +1156,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1181,7 +1193,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1218,7 +1230,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1241,7 +1253,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1264,7 +1276,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -1284,7 +1296,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1304,7 +1316,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1330,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1353,7 +1365,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1373,7 +1385,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1393,7 +1405,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1418,11 +1430,11 @@
       <c r="O13">
         <v>600</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -1442,7 +1454,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -1462,7 +1474,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1485,7 +1497,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1505,7 +1517,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1526,6 +1538,32 @@
       </c>
       <c r="H18">
         <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -1538,7 +1576,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3283,7 +3321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB42B24B-1FF3-4D04-ABC3-37C8B4C6ACE7}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3345,7 +3383,7 @@
         <v>0.59046130291978205</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:G66" si="0">MIN(1,MAX(0,B3*(1+0.2*COS(A3*PI()/9))))</f>
+        <f t="shared" ref="F3:F66" si="0">MIN(1,MAX(0,B3*(1+0.2*COS(A3*PI()/9))))</f>
         <v>1</v>
       </c>
     </row>
@@ -4689,7 +4727,7 @@
         <v>7.1915703235945705E-2</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:G97" si="1">MIN(1,MAX(0,B67*(1+0.2*COS(A67*PI()/9))))</f>
+        <f t="shared" ref="F67:F97" si="1">MIN(1,MAX(0,B67*(1+0.2*COS(A67*PI()/9))))</f>
         <v>0.29399262638535623</v>
       </c>
     </row>
@@ -5329,12 +5367,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068757AD89D0841429F5831BBC6267AC1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e521892cf07d8fee7d1fab9fe3aaa83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c" xmlns:ns4="53f6e7f0-9e34-4545-9b50-e54ccadfb78a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ffc55c83d6521c05fad87c69f289641" ns3:_="" ns4:_="">
     <xsd:import namespace="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c"/>
@@ -5543,6 +5575,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5553,15 +5591,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1016DCAE-9D9F-40DE-A38A-1587953D2A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5580,6 +5609,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
added losses to storage restructure terminal construction (only split terminal into in/out if necessary)
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327E909B-DD31-40F5-B2B7-84DB7DF41425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFDBBE4-D610-4761-896F-BA42A4A66BB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9252" yWindow="252" windowWidth="18888" windowHeight="16392" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="11580" yWindow="480" windowWidth="18888" windowHeight="16392" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -1069,7 +1069,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1185,12 +1185,12 @@
         <v>0.05</v>
       </c>
       <c r="M3">
-        <f>1/30</f>
-        <v>3.3333333333333333E-2</v>
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="N3">
-        <f>1/30</f>
-        <v>3.3333333333333333E-2</v>
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -1222,12 +1222,12 @@
         <v>0.05</v>
       </c>
       <c r="M4">
-        <f>1/30</f>
-        <v>3.3333333333333333E-2</v>
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="N4">
-        <f>1/30</f>
-        <v>3.3333333333333333E-2</v>
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -1485,7 +1485,7 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1548,7 +1548,7 @@
         <v>84</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>5</v>
@@ -1560,7 +1560,7 @@
         <v>85</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P19">
         <v>2.5</v>
@@ -1657,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E6B22F-D4D7-489D-AE2A-F030E504A301}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2178,7 +2178,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.79261292299999997</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2195,7 +2195,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.797846053</v>
+        <v>0.24</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3321,7 +3321,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB42B24B-1FF3-4D04-ABC3-37C8B4C6ACE7}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4001,7 +4003,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.21235948018265505</v>
+        <v>0.73</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -4014,7 +4016,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>0.2049843128338521</v>
+        <v>0.70464736606062806</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
corrected energy storage equation
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE175899-4D70-4343-A9D5-9103C2F17698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C220B6-C1D0-42A6-A376-E99105328EEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="480" windowWidth="18888" windowHeight="16392" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="5124" yWindow="192" windowWidth="23508" windowHeight="16356" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -1069,7 +1069,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1560,7 +1560,7 @@
         <v>85</v>
       </c>
       <c r="H19">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="P19">
         <v>2.5</v>
@@ -5369,6 +5369,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068757AD89D0841429F5831BBC6267AC1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e521892cf07d8fee7d1fab9fe3aaa83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c" xmlns:ns4="53f6e7f0-9e34-4545-9b50-e54ccadfb78a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ffc55c83d6521c05fad87c69f289641" ns3:_="" ns4:_="">
     <xsd:import namespace="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c"/>
@@ -5577,12 +5583,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5593,6 +5593,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1016DCAE-9D9F-40DE-A38A-1587953D2A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5611,15 +5620,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added petroleum, oil, water networks (energy transport only) Misc modifications
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C220B6-C1D0-42A6-A376-E99105328EEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A471137-CE39-403E-A423-65F32CB8751D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5124" yWindow="192" windowWidth="23508" windowHeight="16356" activeTab="2" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="2016" yWindow="336" windowWidth="23508" windowHeight="16356" activeTab="3" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="88">
   <si>
     <t>id</t>
   </si>
@@ -154,12 +154,6 @@
     <t>nodeTo</t>
   </si>
   <si>
-    <t>gaspressure_in</t>
-  </si>
-  <si>
-    <t>gaspressure_out</t>
-  </si>
-  <si>
     <t>model</t>
   </si>
   <si>
@@ -241,12 +235,6 @@
     <t>CO2_price</t>
   </si>
   <si>
-    <t>export_gas</t>
-  </si>
-  <si>
-    <t>export_el</t>
-  </si>
-  <si>
     <t>source_el</t>
   </si>
   <si>
@@ -299,6 +287,21 @@
   </si>
   <si>
     <t>Emax</t>
+  </si>
+  <si>
+    <t>sink_gas</t>
+  </si>
+  <si>
+    <t>pressure.gas.in</t>
+  </si>
+  <si>
+    <t>pressure.gas.out</t>
+  </si>
+  <si>
+    <t>max_pressure_deviation</t>
+  </si>
+  <si>
+    <t>max terminal pressure deviation from nominal values</t>
   </si>
 </sst>
 </file>
@@ -662,7 +665,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,10 +691,10 @@
         <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -739,7 +742,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -779,7 +782,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B6">
         <v>-1.2</v>
@@ -839,13 +842,13 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>12</v>
@@ -885,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -911,7 +914,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -929,7 +932,7 @@
         <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -940,7 +943,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -963,7 +966,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -986,7 +989,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1041,7 +1044,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1068,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB3A90-DDA6-4778-8302-DAD5F7252115}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,34 +1103,34 @@
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
         <v>46</v>
       </c>
-      <c r="I1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K1" t="s">
-        <v>48</v>
-      </c>
       <c r="L1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="N1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="O1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="Q1" t="s">
         <v>12</v>
@@ -1150,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H2">
         <v>0.5</v>
@@ -1161,7 +1164,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1173,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1198,7 +1201,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1210,7 +1213,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -1247,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H5">
         <v>1E-3</v>
@@ -1270,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H6">
         <v>4.0000000000000001E-3</v>
@@ -1278,7 +1281,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
         <v>35</v>
@@ -1293,7 +1296,7 @@
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -1313,7 +1316,7 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -1336,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1359,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H10">
         <v>3</v>
@@ -1382,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -1402,7 +1405,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -1416,7 +1419,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E13">
         <v>5000</v>
@@ -1425,18 +1428,18 @@
         <v>5000</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O13">
         <v>600</v>
       </c>
       <c r="Q13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
         <v>31</v>
@@ -1451,12 +1454,12 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
         <v>32</v>
@@ -1471,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -1491,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I16">
         <v>30</v>
@@ -1514,7 +1517,7 @@
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -1534,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H18">
         <v>3</v>
@@ -1545,7 +1548,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1557,7 +1560,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H19">
         <v>0.9</v>
@@ -1573,24 +1576,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F6EB10-AB47-4D11-878D-7EA50574CBA2}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
@@ -1598,29 +1601,29 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2">
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3">
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -1628,24 +1631,35 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7">
+        <v>0.1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1665,19 +1679,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
         <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -3329,22 +3343,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
         <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -5369,9 +5383,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5584,19 +5601,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5621,9 +5634,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>